<commit_message>
1.修改excel.yaml配置，修改键  field_type_row 为  field_switch_row，拆分  field_name_rows为  lang_key_rows 和  file_key_rows。 2.调整各编程语言生成模板。 3.增加忽略目录。
</commit_message>
<xml_diff>
--- a/res/source/cfg_building_new.xlsx
+++ b/res/source/cfg_building_new.xlsx
@@ -16,12 +16,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data_Sheet1!#REF!</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="299">
   <si>
     <t>建筑</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1076,6 +1075,98 @@
   </si>
   <si>
     <t>0,0,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>building_type_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>promotion_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>layoutX_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type_idx_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gateX_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gateY_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>terrain_flags_j</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>supply_population_type_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isDoor_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc1_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc2_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc3_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f1_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f2_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f3_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f4_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f5_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f6_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f7_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f8_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f9_j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f10_j</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1738,13 +1829,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W20"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="J7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2140,115 +2231,115 @@
       </c>
     </row>
     <row r="7" spans="1:23" s="33" customFormat="1">
-      <c r="A7" s="29">
+      <c r="A7" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>283</v>
+      </c>
+      <c r="I7" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="J7" s="30" t="s">
+        <v>285</v>
+      </c>
+      <c r="K7" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="L7" s="32" t="s">
+        <v>287</v>
+      </c>
+      <c r="M7" s="32" t="s">
+        <v>288</v>
+      </c>
+      <c r="N7" s="33" t="s">
+        <v>289</v>
+      </c>
+      <c r="O7" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="P7" s="33" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q7" s="33" t="s">
+        <v>292</v>
+      </c>
+      <c r="R7" s="33" t="s">
+        <v>293</v>
+      </c>
+      <c r="S7" s="33" t="s">
+        <v>294</v>
+      </c>
+      <c r="T7" s="33" t="s">
+        <v>295</v>
+      </c>
+      <c r="U7" s="33" t="s">
+        <v>296</v>
+      </c>
+      <c r="V7" s="33" t="s">
+        <v>297</v>
+      </c>
+      <c r="W7" s="33" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" s="33" customFormat="1">
+      <c r="A8" s="29">
         <v>99</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B8" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="C7" s="32">
-        <v>0</v>
-      </c>
-      <c r="D7" s="32">
-        <v>0</v>
-      </c>
-      <c r="E7" s="32">
-        <v>0</v>
-      </c>
-      <c r="F7" s="32">
+      <c r="C8" s="32">
+        <v>0</v>
+      </c>
+      <c r="D8" s="32">
+        <v>0</v>
+      </c>
+      <c r="E8" s="32">
+        <v>0</v>
+      </c>
+      <c r="F8" s="32">
         <v>3.5</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G8" s="32">
         <v>-2.2999999999999998</v>
       </c>
-      <c r="H7" s="26">
-        <v>0</v>
-      </c>
-      <c r="I7" s="30">
-        <v>0</v>
-      </c>
-      <c r="J7" s="30">
-        <v>0</v>
-      </c>
-      <c r="K7" s="32" t="s">
+      <c r="H8" s="26">
+        <v>0</v>
+      </c>
+      <c r="I8" s="30">
+        <v>0</v>
+      </c>
+      <c r="J8" s="30">
+        <v>0</v>
+      </c>
+      <c r="K8" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="L7" s="32" t="s">
+      <c r="L8" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="M7" s="32" t="s">
+      <c r="M8" s="32" t="s">
         <v>190</v>
-      </c>
-      <c r="N7" s="33" t="s">
-        <v>209</v>
-      </c>
-      <c r="O7" s="33" t="s">
-        <v>213</v>
-      </c>
-      <c r="P7" s="33" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q7" s="33" t="s">
-        <v>235</v>
-      </c>
-      <c r="R7" s="33" t="s">
-        <v>236</v>
-      </c>
-      <c r="S7" s="33" t="s">
-        <v>237</v>
-      </c>
-      <c r="T7" s="33" t="s">
-        <v>238</v>
-      </c>
-      <c r="U7" s="33" t="s">
-        <v>239</v>
-      </c>
-      <c r="V7" s="33" t="s">
-        <v>256</v>
-      </c>
-      <c r="W7" s="33" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" ht="17.25">
-      <c r="A8" s="30">
-        <v>101</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="30">
-        <v>1</v>
-      </c>
-      <c r="D8" s="30">
-        <v>1</v>
-      </c>
-      <c r="E8" s="30">
-        <v>1</v>
-      </c>
-      <c r="F8" s="54">
-        <v>-2147483647</v>
-      </c>
-      <c r="G8" s="54">
-        <v>-2147483647</v>
-      </c>
-      <c r="H8" s="55">
-        <v>-2147483648</v>
-      </c>
-      <c r="I8" s="30">
-        <v>-32768</v>
-      </c>
-      <c r="J8" s="30">
-        <v>1</v>
-      </c>
-      <c r="K8" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="M8" s="32" t="s">
-        <v>191</v>
       </c>
       <c r="N8" s="33" t="s">
         <v>209</v>
@@ -2272,54 +2363,54 @@
         <v>238</v>
       </c>
       <c r="U8" s="33" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="V8" s="33" t="s">
         <v>256</v>
       </c>
       <c r="W8" s="33" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="17.25">
       <c r="A9" s="30">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="30">
-        <v>127</v>
+        <v>1</v>
       </c>
       <c r="D9" s="30">
-        <v>32767</v>
-      </c>
-      <c r="E9" s="56">
-        <v>2147483647</v>
+        <v>1</v>
+      </c>
+      <c r="E9" s="30">
+        <v>1</v>
       </c>
       <c r="F9" s="54">
-        <v>2147483646</v>
+        <v>-2147483647</v>
       </c>
       <c r="G9" s="54">
-        <v>2147483646</v>
+        <v>-2147483647</v>
       </c>
       <c r="H9" s="55">
-        <v>2147483647</v>
+        <v>-2147483648</v>
       </c>
       <c r="I9" s="30">
-        <v>32767</v>
+        <v>-32768</v>
       </c>
       <c r="J9" s="30">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K9" s="30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L9" s="30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M9" s="32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N9" s="33" t="s">
         <v>209</v>
@@ -2343,54 +2434,54 @@
         <v>238</v>
       </c>
       <c r="U9" s="33" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="V9" s="33" t="s">
         <v>256</v>
       </c>
       <c r="W9" s="33" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="17.25">
       <c r="A10" s="30">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="30">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D10" s="30">
-        <v>32768</v>
+        <v>32767</v>
       </c>
       <c r="E10" s="56">
-        <v>2147483648</v>
-      </c>
-      <c r="F10" s="29">
+        <v>2147483647</v>
+      </c>
+      <c r="F10" s="54">
+        <v>2147483646</v>
+      </c>
+      <c r="G10" s="54">
+        <v>2147483646</v>
+      </c>
+      <c r="H10" s="55">
+        <v>2147483647</v>
+      </c>
+      <c r="I10" s="30">
+        <v>32767</v>
+      </c>
+      <c r="J10" s="30">
         <v>-1</v>
       </c>
-      <c r="G10" s="29">
-        <v>-1</v>
-      </c>
-      <c r="H10" s="29">
-        <v>-1</v>
-      </c>
-      <c r="I10" s="30">
-        <v>-1</v>
-      </c>
-      <c r="J10" s="30">
-        <v>126</v>
-      </c>
       <c r="K10" s="30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L10" s="30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M10" s="32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N10" s="33" t="s">
         <v>209</v>
@@ -2414,54 +2505,54 @@
         <v>238</v>
       </c>
       <c r="U10" s="33" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="V10" s="33" t="s">
         <v>256</v>
       </c>
       <c r="W10" s="33" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="17.25">
       <c r="A11" s="30">
-        <v>201</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>135</v>
+        <v>103</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>4</v>
       </c>
       <c r="C11" s="30">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D11" s="30">
-        <v>32769</v>
+        <v>32768</v>
       </c>
       <c r="E11" s="56">
-        <v>2147483649</v>
+        <v>2147483648</v>
       </c>
       <c r="F11" s="29">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G11" s="29">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H11" s="29">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I11" s="30">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J11" s="30">
-        <v>127</v>
-      </c>
-      <c r="K11" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="L11" s="34" t="s">
-        <v>135</v>
+        <v>126</v>
+      </c>
+      <c r="K11" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="L11" s="30" t="s">
+        <v>4</v>
       </c>
       <c r="M11" s="32" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N11" s="33" t="s">
         <v>209</v>
@@ -2485,54 +2576,54 @@
         <v>238</v>
       </c>
       <c r="U11" s="33" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="V11" s="33" t="s">
         <v>256</v>
       </c>
       <c r="W11" s="33" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="17.25">
       <c r="A12" s="30">
-        <v>202</v>
-      </c>
-      <c r="B12" s="35" t="s">
-        <v>5</v>
+        <v>201</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>135</v>
       </c>
       <c r="C12" s="30">
-        <v>255</v>
+        <v>129</v>
       </c>
       <c r="D12" s="30">
-        <v>65535</v>
+        <v>32769</v>
       </c>
       <c r="E12" s="56">
-        <v>4294967295</v>
-      </c>
-      <c r="F12" s="54">
-        <v>-2147483647</v>
-      </c>
-      <c r="G12" s="54">
-        <v>-2147483647</v>
-      </c>
-      <c r="H12" s="55">
-        <v>-2147483648</v>
+        <v>2147483649</v>
+      </c>
+      <c r="F12" s="29">
+        <v>1</v>
+      </c>
+      <c r="G12" s="29">
+        <v>1</v>
+      </c>
+      <c r="H12" s="29">
+        <v>1</v>
       </c>
       <c r="I12" s="30">
-        <v>-32767</v>
+        <v>1</v>
       </c>
       <c r="J12" s="30">
-        <v>-128</v>
-      </c>
-      <c r="K12" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="L12" s="35" t="s">
-        <v>5</v>
+        <v>127</v>
+      </c>
+      <c r="K12" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="L12" s="34" t="s">
+        <v>135</v>
       </c>
       <c r="M12" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N12" s="33" t="s">
         <v>209</v>
@@ -2556,21 +2647,21 @@
         <v>238</v>
       </c>
       <c r="U12" s="33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="V12" s="33" t="s">
         <v>256</v>
       </c>
       <c r="W12" s="33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="17.25">
       <c r="A13" s="30">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="30">
         <v>255</v>
@@ -2582,28 +2673,28 @@
         <v>4294967295</v>
       </c>
       <c r="F13" s="54">
-        <v>2147483646</v>
+        <v>-2147483647</v>
       </c>
       <c r="G13" s="54">
-        <v>2147483646</v>
+        <v>-2147483647</v>
       </c>
       <c r="H13" s="55">
-        <v>2147483647</v>
+        <v>-2147483648</v>
       </c>
       <c r="I13" s="30">
-        <v>32766</v>
+        <v>-32767</v>
       </c>
       <c r="J13" s="30">
-        <v>-127</v>
+        <v>-128</v>
       </c>
       <c r="K13" s="35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L13" s="35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M13" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N13" s="33" t="s">
         <v>209</v>
@@ -2627,54 +2718,54 @@
         <v>238</v>
       </c>
       <c r="U13" s="33" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="V13" s="33" t="s">
         <v>256</v>
       </c>
       <c r="W13" s="33" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="17.25">
       <c r="A14" s="30">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="30">
-        <v>1</v>
+        <v>255</v>
       </c>
       <c r="D14" s="30">
-        <v>5</v>
-      </c>
-      <c r="E14" s="30">
-        <v>20401</v>
-      </c>
-      <c r="F14" s="30">
-        <v>2</v>
-      </c>
-      <c r="G14" s="30">
-        <v>2</v>
-      </c>
-      <c r="H14" s="29">
-        <v>458894</v>
-      </c>
-      <c r="I14" s="24">
-        <v>0</v>
+        <v>65535</v>
+      </c>
+      <c r="E14" s="56">
+        <v>4294967295</v>
+      </c>
+      <c r="F14" s="54">
+        <v>2147483646</v>
+      </c>
+      <c r="G14" s="54">
+        <v>2147483646</v>
+      </c>
+      <c r="H14" s="55">
+        <v>2147483647</v>
+      </c>
+      <c r="I14" s="30">
+        <v>32766</v>
       </c>
       <c r="J14" s="30">
-        <v>1</v>
+        <v>-127</v>
       </c>
       <c r="K14" s="35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L14" s="35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M14" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N14" s="33" t="s">
         <v>209</v>
@@ -2698,30 +2789,30 @@
         <v>238</v>
       </c>
       <c r="U14" s="33" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="V14" s="33" t="s">
         <v>256</v>
       </c>
       <c r="W14" s="33" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="17.25">
       <c r="A15" s="30">
-        <v>301</v>
+        <v>204</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="35" t="s">
-        <v>148</v>
+        <v>7</v>
+      </c>
+      <c r="C15" s="30">
+        <v>1</v>
       </c>
       <c r="D15" s="30">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" s="30">
-        <v>30101</v>
+        <v>20401</v>
       </c>
       <c r="F15" s="30">
         <v>2</v>
@@ -2733,19 +2824,19 @@
         <v>458894</v>
       </c>
       <c r="I15" s="24">
-        <v>234</v>
+        <v>0</v>
       </c>
       <c r="J15" s="30">
         <v>1</v>
       </c>
       <c r="K15" s="35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L15" s="35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M15" s="32" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N15" s="33" t="s">
         <v>209</v>
@@ -2769,54 +2860,54 @@
         <v>238</v>
       </c>
       <c r="U15" s="33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="V15" s="33" t="s">
         <v>256</v>
       </c>
       <c r="W15" s="33" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" s="38" customFormat="1" ht="17.25">
-      <c r="A16" s="36">
-        <v>401</v>
-      </c>
-      <c r="B16" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="D16" s="36">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="17.25">
+      <c r="A16" s="30">
+        <v>301</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" s="30">
         <v>6</v>
       </c>
-      <c r="E16" s="36">
-        <v>40101</v>
-      </c>
-      <c r="F16" s="36">
-        <v>-5.6</v>
-      </c>
-      <c r="G16" s="36">
-        <v>2.2999999999999998</v>
+      <c r="E16" s="30">
+        <v>30101</v>
+      </c>
+      <c r="F16" s="30">
+        <v>2</v>
+      </c>
+      <c r="G16" s="30">
+        <v>2</v>
       </c>
       <c r="H16" s="29">
         <v>458894</v>
       </c>
-      <c r="I16" s="39">
-        <v>0</v>
-      </c>
-      <c r="J16" s="36">
-        <v>1</v>
-      </c>
-      <c r="K16" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="L16" s="37" t="s">
-        <v>9</v>
+      <c r="I16" s="24">
+        <v>234</v>
+      </c>
+      <c r="J16" s="30">
+        <v>1</v>
+      </c>
+      <c r="K16" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="L16" s="35" t="s">
+        <v>8</v>
       </c>
       <c r="M16" s="32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N16" s="33" t="s">
         <v>209</v>
@@ -2840,36 +2931,36 @@
         <v>238</v>
       </c>
       <c r="U16" s="33" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="V16" s="33" t="s">
         <v>256</v>
       </c>
       <c r="W16" s="33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:23" s="38" customFormat="1" ht="17.25">
       <c r="A17" s="36">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D17" s="36">
         <v>6</v>
       </c>
       <c r="E17" s="36">
-        <v>40201</v>
+        <v>40101</v>
       </c>
       <c r="F17" s="36">
-        <v>2</v>
+        <v>-5.6</v>
       </c>
       <c r="G17" s="36">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H17" s="29">
         <v>458894</v>
@@ -2881,13 +2972,13 @@
         <v>1</v>
       </c>
       <c r="K17" s="37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L17" s="37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M17" s="32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N17" s="33" t="s">
         <v>209</v>
@@ -2911,36 +3002,36 @@
         <v>238</v>
       </c>
       <c r="U17" s="33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="V17" s="33" t="s">
         <v>256</v>
       </c>
       <c r="W17" s="33" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:23" s="38" customFormat="1" ht="17.25">
       <c r="A18" s="36">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="37" t="s">
         <v>128</v>
       </c>
       <c r="D18" s="36">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18" s="36">
-        <v>40301</v>
+        <v>40201</v>
       </c>
       <c r="F18" s="36">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G18" s="36">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H18" s="29">
         <v>458894</v>
@@ -2952,13 +3043,13 @@
         <v>1</v>
       </c>
       <c r="K18" s="37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L18" s="37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M18" s="32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N18" s="33" t="s">
         <v>209</v>
@@ -2982,36 +3073,36 @@
         <v>238</v>
       </c>
       <c r="U18" s="33" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V18" s="33" t="s">
         <v>256</v>
       </c>
       <c r="W18" s="33" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19" spans="1:23" s="38" customFormat="1" ht="17.25">
       <c r="A19" s="36">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" s="37" t="s">
         <v>128</v>
       </c>
       <c r="D19" s="36">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E19" s="36">
-        <v>40401</v>
+        <v>40301</v>
       </c>
       <c r="F19" s="36">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G19" s="36">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H19" s="29">
         <v>458894</v>
@@ -3023,13 +3114,13 @@
         <v>1</v>
       </c>
       <c r="K19" s="37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L19" s="37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M19" s="32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N19" s="33" t="s">
         <v>209</v>
@@ -3053,30 +3144,30 @@
         <v>238</v>
       </c>
       <c r="U19" s="33" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="V19" s="33" t="s">
         <v>256</v>
       </c>
       <c r="W19" s="33" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:23" s="38" customFormat="1" ht="17.25">
       <c r="A20" s="36">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" s="37" t="s">
         <v>128</v>
       </c>
       <c r="D20" s="36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E20" s="36">
-        <v>40501</v>
+        <v>40401</v>
       </c>
       <c r="F20" s="36">
         <v>2</v>
@@ -3094,13 +3185,13 @@
         <v>1</v>
       </c>
       <c r="K20" s="37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L20" s="37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M20" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N20" s="33" t="s">
         <v>209</v>
@@ -3124,12 +3215,83 @@
         <v>238</v>
       </c>
       <c r="U20" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="V20" s="33" t="s">
         <v>256</v>
       </c>
       <c r="W20" s="33" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" s="38" customFormat="1" ht="17.25">
+      <c r="A21" s="36">
+        <v>405</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21" s="36">
+        <v>4</v>
+      </c>
+      <c r="E21" s="36">
+        <v>40501</v>
+      </c>
+      <c r="F21" s="36">
+        <v>2</v>
+      </c>
+      <c r="G21" s="36">
+        <v>2</v>
+      </c>
+      <c r="H21" s="29">
+        <v>458894</v>
+      </c>
+      <c r="I21" s="39">
+        <v>0</v>
+      </c>
+      <c r="J21" s="36">
+        <v>1</v>
+      </c>
+      <c r="K21" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="M21" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="N21" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="O21" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="P21" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q21" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="R21" s="33" t="s">
+        <v>236</v>
+      </c>
+      <c r="S21" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="T21" s="33" t="s">
+        <v>238</v>
+      </c>
+      <c r="U21" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="V21" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="W21" s="33" t="s">
         <v>270</v>
       </c>
     </row>

</xml_diff>